<commit_message>
removed some commente dout code
</commit_message>
<xml_diff>
--- a/excelNew.xlsx
+++ b/excelNew.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Willi\Desktop\CS481\TARGEST.Final-1.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BEA34A9F-B242-4DB9-9CD6-C8826468291A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1B9AF2A3-9B7F-4B4C-A604-3A895FCC6B42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="15" yWindow="15" windowWidth="19185" windowHeight="10065" xr2:uid="{3A49F9AD-A89C-4EE8-B55D-9DA77475E3DF}"/>
+    <workbookView xWindow="15" yWindow="15" windowWidth="19185" windowHeight="10065" xr2:uid="{9BD13FF8-97EA-40E0-B6B6-2D8866A0D43B}"/>
   </bookViews>
   <sheets>
     <sheet name="ReportNew" sheetId="1" r:id="rId1"/>
@@ -863,7 +863,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F364022-53A4-4C4F-9CB5-1A3115D99F98}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDF8656B-CE5F-401B-8EC2-4E5C061345AA}">
   <dimension ref="A1:G280"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Newest version of gui
</commit_message>
<xml_diff>
--- a/excelNew.xlsx
+++ b/excelNew.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Willi\Desktop\CS481\TARGEST.Final-1.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CC4DA647-7316-4E1F-B847-42695E8F2359}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{65935CFC-57C4-4033-B597-B56E0B521E8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="15" windowWidth="19185" windowHeight="10065" xr2:uid="{70D49934-2196-4EE2-9595-21CD0245E686}"/>
+    <workbookView xWindow="15" yWindow="15" windowWidth="19185" windowHeight="10065" xr2:uid="{BDDAE5B0-18DE-47B3-AB2E-9E5B7F5C98AB}"/>
   </bookViews>
   <sheets>
     <sheet name="ReportNew" sheetId="1" r:id="rId1"/>
@@ -381,7 +381,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0B0F8F7-8383-49A9-B8F7-B5A6102040C3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16E2FB65-E0D4-4A50-878A-F773CE4C45C2}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
changed Gui to Tandem blue
</commit_message>
<xml_diff>
--- a/excelNew.xlsx
+++ b/excelNew.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Willi\Desktop\CS481\TARGEST.Final-1.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{86D5E620-20BD-4089-A0CB-F60DFCE2D640}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7C9A9B83-40A0-4580-B601-380F512E70FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10276" xr2:uid="{47F660EE-C8F7-42F3-A807-04A7F3E0C9F6}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10276" xr2:uid="{2FB51011-552C-4BAF-B72D-F3B15713FD0B}"/>
   </bookViews>
   <sheets>
     <sheet name="ReportNew" sheetId="1" r:id="rId1"/>
@@ -569,7 +569,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -864,20 +864,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6FFA1CC-2863-43C8-828F-588AA84C2DE7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55A754A2-D00B-4E4D-8CF1-6BDBFE719EC1}">
   <dimension ref="A1:G280"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="14.46484375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.3984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.796875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.86328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.3984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.1328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.06640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.45">
@@ -2522,6 +2522,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>